<commit_message>
Uploading new version of Gantt File
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/thomas_chapman2_griffithuni_edu_au/Documents/2810 Software Tech/ASSIGNMENT/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{9440CBC7-0273-4BA5-9F39-FB275DE7D8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47B54B2E-AFCB-481D-AEB0-2921EF24DEEA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,90 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>PERIODS</t>
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -230,40 +153,91 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
+    <t>1.1 Establishing team communication pathways</t>
+  </si>
+  <si>
+    <t>NSW Traffic Penalty Data Prog (Gantt Chart)</t>
+  </si>
+  <si>
+    <t>1.3 Producing a scope</t>
+  </si>
+  <si>
+    <t>1.4 WBS Structure</t>
+  </si>
+  <si>
+    <t>Stage 1 (Planning)</t>
+  </si>
+  <si>
+    <t>Stage 2 (Design)</t>
+  </si>
+  <si>
+    <t>1.2 Understanding / researching current systems</t>
+  </si>
+  <si>
+    <t>1.5 Development of Gantt Chart</t>
+  </si>
+  <si>
+    <t>2.1 Create an idea / statement</t>
+  </si>
+  <si>
+    <t>2.2 Establish the project requirements</t>
+  </si>
+  <si>
+    <t>2.3 Establish software places in practice</t>
+  </si>
+  <si>
+    <t>2.4 Establish software places where not in practice</t>
+  </si>
+  <si>
+    <t>2.5 Establish system components</t>
+  </si>
+  <si>
+    <t>2.6 Template / Wireframe</t>
+  </si>
+  <si>
+    <t>Stage 3 (Software Development)</t>
+  </si>
+  <si>
+    <t>Stage 4 (Implementation)</t>
+  </si>
+  <si>
+    <t>Stage 5 (Closing)</t>
+  </si>
+  <si>
+    <t>5.1.1 Final Reporting</t>
+  </si>
+  <si>
+    <t>3.2 Implementing external software (PANDAS Software)</t>
+  </si>
+  <si>
+    <t>3.3 Input data from dataset</t>
+  </si>
+  <si>
+    <t>3.4 Construct data into readable form</t>
+  </si>
+  <si>
+    <t>3.5 Build GUI</t>
+  </si>
+  <si>
+    <t>4.1 Training of end users</t>
+  </si>
+  <si>
+    <t>4.2 Updates / Status on system operations</t>
+  </si>
+  <si>
+    <t>4.3 Update any possible information / Bug fixing</t>
+  </si>
+  <si>
+    <t>4.4 User support and help documentation</t>
+  </si>
+  <si>
+    <t>3.1 Allocation for software design leader (Unit Coding)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,12 +592,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -636,178 +646,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -824,15 +685,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
         <vertical/>
         <horizontal/>
       </border>
@@ -1189,33 +1041,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="46.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1223,82 +1075,82 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="K2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="Q2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="V2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="35"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>36</v>
+      <c r="AI2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1323,13 +1175,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="38"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1511,326 +1363,479 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6</v>
+      </c>
       <c r="G10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C11" s="7">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="C13" s="7">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="C14" s="7">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="C15" s="9">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7">
+        <v>3</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="C16" s="7">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="C17" s="7">
+        <v>16</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="C18" s="7">
+        <v>20</v>
+      </c>
+      <c r="D18" s="7">
+        <v>11</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C19" s="7">
+        <v>20</v>
+      </c>
+      <c r="D19" s="7">
+        <v>10</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C20" s="7">
+        <v>20</v>
+      </c>
+      <c r="D20" s="7">
+        <v>10</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C21" s="7">
+        <v>22</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C22" s="7">
+        <v>23</v>
+      </c>
+      <c r="D22" s="7">
+        <v>6</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="7">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>8</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="C24" s="7">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7">
+        <v>6</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="C25" s="7">
+        <v>31</v>
+      </c>
+      <c r="D25" s="7">
+        <v>3</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="C26" s="7">
+        <v>32</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="C27" s="7">
+        <v>33</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C28" s="7">
+        <v>33</v>
+      </c>
+      <c r="D28" s="7">
+        <v>5</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C29" s="7">
+        <v>37</v>
+      </c>
+      <c r="D29" s="7">
+        <v>5</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C30" s="7">
+        <v>37</v>
+      </c>
+      <c r="D30" s="7">
+        <v>5</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1839,101 +1844,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
-        <v>41</v>
-      </c>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1949,56 +1922,56 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
+  <conditionalFormatting sqref="J6:BO7 K8:BO8 O9:BO9 P10:BO10 H11:BO39 Q5:BO5">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 I7 H10:I10" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 J10:M10 H6:I6 H7:H9 I8:J8 I9:M9 H5:P5" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2 O10 N9:N10" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>